<commit_message>
minor tweaks & audio implementation
</commit_message>
<xml_diff>
--- a/chromalgama balance.xlsx
+++ b/chromalgama balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diabr\Documents\chromalgama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE7AFD6-6047-404F-898F-241B812B0526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B574728E-A2B2-4DCD-8CFC-978BF97E7C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="64">
   <si>
     <t>Т1</t>
   </si>
@@ -127,13 +127,103 @@
   </si>
   <si>
     <t>30.87</t>
+  </si>
+  <si>
+    <t>Звуковое сопровождение</t>
+  </si>
+  <si>
+    <t>Музыка в меню</t>
+  </si>
+  <si>
+    <t>Музыка в бою</t>
+  </si>
+  <si>
+    <t>Гвоздемет</t>
+  </si>
+  <si>
+    <t>Сварочный луч</t>
+  </si>
+  <si>
+    <t>Оптический пар</t>
+  </si>
+  <si>
+    <t>Пороховая турель</t>
+  </si>
+  <si>
+    <t>Разрядник</t>
+  </si>
+  <si>
+    <t>Плазменная бомба</t>
+  </si>
+  <si>
+    <t>Микроволновая турель</t>
+  </si>
+  <si>
+    <t>УФ-лазер</t>
+  </si>
+  <si>
+    <t>Сброс дрона</t>
+  </si>
+  <si>
+    <t>Сборка дрона</t>
+  </si>
+  <si>
+    <t>Нейтронный луч</t>
+  </si>
+  <si>
+    <t>Антиматериальный луч</t>
+  </si>
+  <si>
+    <t>МРП</t>
+  </si>
+  <si>
+    <t>Сброс истребителя</t>
+  </si>
+  <si>
+    <t>Выпуск из ангара</t>
+  </si>
+  <si>
+    <t>ИК-луч</t>
+  </si>
+  <si>
+    <t>Газовый луч</t>
+  </si>
+  <si>
+    <t>Термоядерный луч</t>
+  </si>
+  <si>
+    <t>Главный двигатель</t>
+  </si>
+  <si>
+    <t>Поворотные ускорители</t>
+  </si>
+  <si>
+    <t>Взрыв</t>
+  </si>
+  <si>
+    <t>Нажатие на кнопку</t>
+  </si>
+  <si>
+    <t>Зависание над кнопкой</t>
+  </si>
+  <si>
+    <t>Звук найден</t>
+  </si>
+  <si>
+    <t>Звук установлен</t>
+  </si>
+  <si>
+    <t>Звук норм</t>
+  </si>
+  <si>
+    <t>Нанесение урона</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,8 +244,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +318,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -235,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -263,6 +371,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -548,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,9 +674,13 @@
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -586,8 +702,21 @@
       <c r="G1" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -609,8 +738,14 @@
       <c r="G2">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -632,8 +767,14 @@
       <c r="G3" s="5">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -655,8 +796,14 @@
       <c r="G4" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="17"/>
+      <c r="I4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -678,8 +825,14 @@
       <c r="G5" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="17"/>
+      <c r="I5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -701,8 +854,14 @@
       <c r="G6" s="16">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="17"/>
+      <c r="I6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -724,8 +883,14 @@
       <c r="G7" s="5">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="17"/>
+      <c r="I7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -747,8 +912,14 @@
       <c r="G8" s="5">
         <v>10.58</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="17"/>
+      <c r="I8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -770,8 +941,14 @@
       <c r="G9" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="17"/>
+      <c r="I9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -793,8 +970,14 @@
       <c r="G10" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="17"/>
+      <c r="I10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -816,8 +999,14 @@
       <c r="G11">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="17"/>
+      <c r="I11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -839,8 +1028,14 @@
       <c r="G12" s="5">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="17"/>
+      <c r="I12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -862,8 +1057,13 @@
       <c r="G13" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="17"/>
+      <c r="I13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -885,8 +1085,13 @@
       <c r="G14" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="17"/>
+      <c r="I14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -908,8 +1113,13 @@
       <c r="G15" s="16">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="17"/>
+      <c r="I15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -931,8 +1141,13 @@
       <c r="G16" s="5">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="17"/>
+      <c r="I16" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -954,8 +1169,13 @@
       <c r="G17" s="5">
         <v>10.58</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="17"/>
+      <c r="I17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -977,8 +1197,13 @@
       <c r="G18" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="17"/>
+      <c r="I18" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>22</v>
       </c>
@@ -1000,8 +1225,13 @@
       <c r="G19" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="17"/>
+      <c r="I19" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1023,8 +1253,13 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="17"/>
+      <c r="I20" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1046,8 +1281,13 @@
       <c r="G21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="17"/>
+      <c r="I21" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1069,8 +1309,14 @@
       <c r="G22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="17"/>
+      <c r="I22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1092,8 +1338,14 @@
       <c r="G23" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="17"/>
+      <c r="I23" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1115,8 +1367,13 @@
       <c r="G24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="17"/>
+      <c r="I24" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1138,8 +1395,13 @@
       <c r="G25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="17"/>
+      <c r="I25" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1161,8 +1423,13 @@
       <c r="G26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="17"/>
+      <c r="I26" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1184,8 +1451,13 @@
       <c r="G27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="17"/>
+      <c r="I27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>23</v>
       </c>
@@ -1207,8 +1479,10 @@
       <c r="G28" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1230,8 +1504,10 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1253,8 +1529,10 @@
       <c r="G30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1276,8 +1554,10 @@
       <c r="G31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1299,8 +1579,10 @@
       <c r="G32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1322,8 +1604,10 @@
       <c r="G33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1345,8 +1629,10 @@
       <c r="G34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1368,8 +1654,10 @@
       <c r="G35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1391,8 +1679,10 @@
       <c r="G36" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>24</v>
       </c>
@@ -1414,8 +1704,10 @@
       <c r="G37" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1437,8 +1729,10 @@
       <c r="G38" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1460,8 +1754,10 @@
       <c r="G39" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1483,8 +1779,10 @@
       <c r="G40" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1506,8 +1804,10 @@
       <c r="G41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1529,8 +1829,10 @@
       <c r="G42" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1552,8 +1854,10 @@
       <c r="G43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1575,8 +1879,10 @@
       <c r="G44" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>7</v>
       </c>

</xml_diff>